<commit_message>
Generated the file for CustomerRich Products Corporation - HQ @ Buffalo, NY in the production server
</commit_message>
<xml_diff>
--- a/Rich Products Corporation - HQ @ Buffalo, NY.xlsx
+++ b/Rich Products Corporation - HQ @ Buffalo, NY.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="297">
   <si>
     <t>Rich Products Corporation - HQ @ Buffalo, NY</t>
   </si>
@@ -1444,6 +1444,18 @@
       <c r="I5" t="s">
         <v>21</v>
       </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
@@ -1470,6 +1482,18 @@
       <c r="I6" t="s">
         <v>21</v>
       </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
@@ -1496,6 +1520,18 @@
       <c r="I7" t="s">
         <v>21</v>
       </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
@@ -1525,6 +1561,18 @@
       <c r="I8" t="s">
         <v>21</v>
       </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
@@ -1554,6 +1602,18 @@
       <c r="I9" t="s">
         <v>21</v>
       </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" t="s">
@@ -1580,6 +1640,18 @@
       <c r="I10" t="s">
         <v>21</v>
       </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" t="s">
@@ -1609,6 +1681,18 @@
       <c r="I11" t="s">
         <v>40</v>
       </c>
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
@@ -1638,6 +1722,18 @@
       <c r="I12" t="s">
         <v>46</v>
       </c>
+      <c r="J12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
@@ -1667,6 +1763,18 @@
       <c r="I13" t="s">
         <v>21</v>
       </c>
+      <c r="J13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
@@ -1694,6 +1802,18 @@
         <v>25</v>
       </c>
       <c r="I14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1748,8 +1868,20 @@
       <c r="I16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1777,8 +1909,20 @@
       <c r="I17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1806,8 +1950,20 @@
       <c r="I18" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1835,8 +1991,20 @@
       <c r="I19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1864,8 +2032,20 @@
       <c r="I20" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1893,8 +2073,20 @@
       <c r="I21" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1922,8 +2114,20 @@
       <c r="I22" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1951,8 +2155,20 @@
       <c r="I23" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1980,8 +2196,20 @@
       <c r="I24" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -2009,8 +2237,20 @@
       <c r="I25" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" t="s">
+        <v>21</v>
+      </c>
+      <c r="M25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -2038,8 +2278,20 @@
       <c r="I26" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" t="s">
+        <v>21</v>
+      </c>
+      <c r="M26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2067,8 +2319,20 @@
       <c r="I27" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -2096,8 +2360,20 @@
       <c r="I28" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" t="s">
+        <v>21</v>
+      </c>
+      <c r="M28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -2125,8 +2401,20 @@
       <c r="I29" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2154,8 +2442,20 @@
       <c r="I30" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -2183,8 +2483,20 @@
       <c r="I31" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -2212,8 +2524,20 @@
       <c r="I32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2241,8 +2565,20 @@
       <c r="I33" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2270,8 +2606,20 @@
       <c r="I34" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2299,8 +2647,20 @@
       <c r="I35" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" t="s">
+        <v>21</v>
+      </c>
+      <c r="M35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2328,8 +2688,20 @@
       <c r="I36" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="J36" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36" t="s">
+        <v>21</v>
+      </c>
+      <c r="M36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2357,8 +2729,20 @@
       <c r="I37" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="J37" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" t="s">
+        <v>21</v>
+      </c>
+      <c r="M37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -2386,8 +2770,20 @@
       <c r="I38" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" t="s">
+        <v>21</v>
+      </c>
+      <c r="L38" t="s">
+        <v>21</v>
+      </c>
+      <c r="M38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -2415,8 +2811,20 @@
       <c r="I39" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="J39" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" t="s">
+        <v>21</v>
+      </c>
+      <c r="L39" t="s">
+        <v>21</v>
+      </c>
+      <c r="M39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -2444,8 +2852,20 @@
       <c r="I40" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="J40" t="s">
+        <v>21</v>
+      </c>
+      <c r="K40" t="s">
+        <v>21</v>
+      </c>
+      <c r="L40" t="s">
+        <v>21</v>
+      </c>
+      <c r="M40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -2473,8 +2893,20 @@
       <c r="I41" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="J41" t="s">
+        <v>21</v>
+      </c>
+      <c r="K41" t="s">
+        <v>21</v>
+      </c>
+      <c r="L41" t="s">
+        <v>21</v>
+      </c>
+      <c r="M41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -2502,8 +2934,20 @@
       <c r="I42" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42" t="s">
+        <v>21</v>
+      </c>
+      <c r="K42" t="s">
+        <v>21</v>
+      </c>
+      <c r="L42" t="s">
+        <v>21</v>
+      </c>
+      <c r="M42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -2531,8 +2975,20 @@
       <c r="I43" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43" t="s">
+        <v>21</v>
+      </c>
+      <c r="K43" t="s">
+        <v>21</v>
+      </c>
+      <c r="L43" t="s">
+        <v>21</v>
+      </c>
+      <c r="M43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -2560,8 +3016,20 @@
       <c r="I44" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="45" spans="1:9">
+      <c r="J44" t="s">
+        <v>21</v>
+      </c>
+      <c r="K44" t="s">
+        <v>21</v>
+      </c>
+      <c r="L44" t="s">
+        <v>21</v>
+      </c>
+      <c r="M44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2589,8 +3057,20 @@
       <c r="I45" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="46" spans="1:9">
+      <c r="J45" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" t="s">
+        <v>21</v>
+      </c>
+      <c r="L45" t="s">
+        <v>21</v>
+      </c>
+      <c r="M45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -2618,8 +3098,20 @@
       <c r="I46" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="J46" t="s">
+        <v>21</v>
+      </c>
+      <c r="K46" t="s">
+        <v>21</v>
+      </c>
+      <c r="L46" t="s">
+        <v>21</v>
+      </c>
+      <c r="M46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -2647,8 +3139,20 @@
       <c r="I47" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" t="s">
+        <v>21</v>
+      </c>
+      <c r="K47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L47" t="s">
+        <v>21</v>
+      </c>
+      <c r="M47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -2675,6 +3179,18 @@
       </c>
       <c r="I48" t="s">
         <v>116</v>
+      </c>
+      <c r="J48" t="s">
+        <v>21</v>
+      </c>
+      <c r="K48" t="s">
+        <v>21</v>
+      </c>
+      <c r="L48" t="s">
+        <v>21</v>
+      </c>
+      <c r="M48" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:19">
@@ -2705,6 +3221,18 @@
       <c r="I49" t="s">
         <v>73</v>
       </c>
+      <c r="J49" t="s">
+        <v>21</v>
+      </c>
+      <c r="K49" t="s">
+        <v>21</v>
+      </c>
+      <c r="L49" t="s">
+        <v>21</v>
+      </c>
+      <c r="M49" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="50" spans="1:19">
       <c r="A50" t="s">
@@ -2734,6 +3262,18 @@
       <c r="I50" t="s">
         <v>192</v>
       </c>
+      <c r="J50" t="s">
+        <v>21</v>
+      </c>
+      <c r="K50" t="s">
+        <v>21</v>
+      </c>
+      <c r="L50" t="s">
+        <v>21</v>
+      </c>
+      <c r="M50" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="51" spans="1:19">
       <c r="A51" t="s">
@@ -2763,6 +3303,18 @@
       <c r="I51" t="s">
         <v>162</v>
       </c>
+      <c r="J51" t="s">
+        <v>21</v>
+      </c>
+      <c r="K51" t="s">
+        <v>21</v>
+      </c>
+      <c r="L51" t="s">
+        <v>21</v>
+      </c>
+      <c r="M51" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="52" spans="1:19">
       <c r="A52" t="s">
@@ -2791,6 +3343,18 @@
       </c>
       <c r="I52" t="s">
         <v>221</v>
+      </c>
+      <c r="J52" t="s">
+        <v>21</v>
+      </c>
+      <c r="K52" t="s">
+        <v>21</v>
+      </c>
+      <c r="L52" t="s">
+        <v>21</v>
+      </c>
+      <c r="M52" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:19">
@@ -2835,6 +3399,18 @@
       <c r="I54" t="s">
         <v>21</v>
       </c>
+      <c r="J54" t="s">
+        <v>21</v>
+      </c>
+      <c r="K54" t="s">
+        <v>21</v>
+      </c>
+      <c r="L54" t="s">
+        <v>21</v>
+      </c>
+      <c r="M54" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="55" spans="1:19">
       <c r="C55" t="s">
@@ -2858,6 +3434,18 @@
       <c r="I55" t="s">
         <v>21</v>
       </c>
+      <c r="J55" t="s">
+        <v>21</v>
+      </c>
+      <c r="K55" t="s">
+        <v>21</v>
+      </c>
+      <c r="L55" t="s">
+        <v>21</v>
+      </c>
+      <c r="M55" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="56" spans="1:19">
       <c r="C56" t="s">
@@ -2879,6 +3467,18 @@
         <v>226</v>
       </c>
       <c r="I56" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" t="s">
+        <v>21</v>
+      </c>
+      <c r="K56" t="s">
+        <v>21</v>
+      </c>
+      <c r="L56" t="s">
+        <v>21</v>
+      </c>
+      <c r="M56" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2901,6 +3501,18 @@
       <c r="I57" t="s">
         <v>21</v>
       </c>
+      <c r="J57" t="s">
+        <v>21</v>
+      </c>
+      <c r="K57" t="s">
+        <v>21</v>
+      </c>
+      <c r="L57" t="s">
+        <v>21</v>
+      </c>
+      <c r="M57" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="58" spans="1:19">
       <c r="D58" t="s">
@@ -2919,6 +3531,18 @@
         <v>226</v>
       </c>
       <c r="I58" t="s">
+        <v>21</v>
+      </c>
+      <c r="J58" t="s">
+        <v>21</v>
+      </c>
+      <c r="K58" t="s">
+        <v>21</v>
+      </c>
+      <c r="L58" t="s">
+        <v>21</v>
+      </c>
+      <c r="M58" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2967,6 +3591,18 @@
       <c r="I60" t="s">
         <v>21</v>
       </c>
+      <c r="J60" t="s">
+        <v>21</v>
+      </c>
+      <c r="K60" t="s">
+        <v>21</v>
+      </c>
+      <c r="L60" t="s">
+        <v>21</v>
+      </c>
+      <c r="M60" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="61" spans="1:19">
       <c r="C61" t="s">
@@ -2988,6 +3624,18 @@
         <v>226</v>
       </c>
       <c r="I61" t="s">
+        <v>21</v>
+      </c>
+      <c r="J61" t="s">
+        <v>21</v>
+      </c>
+      <c r="K61" t="s">
+        <v>21</v>
+      </c>
+      <c r="L61" t="s">
+        <v>21</v>
+      </c>
+      <c r="M61" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3008,6 +3656,18 @@
         <v>245</v>
       </c>
       <c r="I62" t="s">
+        <v>21</v>
+      </c>
+      <c r="J62" t="s">
+        <v>21</v>
+      </c>
+      <c r="K62" t="s">
+        <v>21</v>
+      </c>
+      <c r="L62" t="s">
+        <v>21</v>
+      </c>
+      <c r="M62" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3062,6 +3722,18 @@
       <c r="I64" t="s">
         <v>252</v>
       </c>
+      <c r="J64" t="s">
+        <v>21</v>
+      </c>
+      <c r="K64" t="s">
+        <v>21</v>
+      </c>
+      <c r="L64" t="s">
+        <v>21</v>
+      </c>
+      <c r="M64" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="65" spans="1:19">
       <c r="A65" t="s">
@@ -3091,6 +3763,18 @@
       <c r="I65" t="s">
         <v>252</v>
       </c>
+      <c r="J65" t="s">
+        <v>21</v>
+      </c>
+      <c r="K65" t="s">
+        <v>21</v>
+      </c>
+      <c r="L65" t="s">
+        <v>21</v>
+      </c>
+      <c r="M65" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="66" spans="1:19">
       <c r="A66" t="s">
@@ -3120,6 +3804,18 @@
       <c r="I66" t="s">
         <v>260</v>
       </c>
+      <c r="J66" t="s">
+        <v>21</v>
+      </c>
+      <c r="K66" t="s">
+        <v>21</v>
+      </c>
+      <c r="L66" t="s">
+        <v>21</v>
+      </c>
+      <c r="M66" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="67" spans="1:19">
       <c r="A67" t="s">
@@ -3149,6 +3845,18 @@
       <c r="I67" t="s">
         <v>266</v>
       </c>
+      <c r="J67" t="s">
+        <v>21</v>
+      </c>
+      <c r="K67" t="s">
+        <v>21</v>
+      </c>
+      <c r="L67" t="s">
+        <v>21</v>
+      </c>
+      <c r="M67" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="68" spans="1:19">
       <c r="A68" t="s">
@@ -3178,6 +3886,18 @@
       <c r="I68" t="s">
         <v>266</v>
       </c>
+      <c r="J68" t="s">
+        <v>21</v>
+      </c>
+      <c r="K68" t="s">
+        <v>21</v>
+      </c>
+      <c r="L68" t="s">
+        <v>21</v>
+      </c>
+      <c r="M68" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="69" spans="1:19">
       <c r="A69" t="s">
@@ -3207,6 +3927,18 @@
       <c r="I69" t="s">
         <v>252</v>
       </c>
+      <c r="J69" t="s">
+        <v>21</v>
+      </c>
+      <c r="K69" t="s">
+        <v>21</v>
+      </c>
+      <c r="L69" t="s">
+        <v>21</v>
+      </c>
+      <c r="M69" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="70" spans="1:19">
       <c r="A70" t="s">
@@ -3236,6 +3968,18 @@
       <c r="I70" t="s">
         <v>266</v>
       </c>
+      <c r="J70" t="s">
+        <v>21</v>
+      </c>
+      <c r="K70" t="s">
+        <v>21</v>
+      </c>
+      <c r="L70" t="s">
+        <v>21</v>
+      </c>
+      <c r="M70" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="71" spans="1:19">
       <c r="A71" t="s">
@@ -3265,6 +4009,18 @@
       <c r="I71" t="s">
         <v>252</v>
       </c>
+      <c r="J71" t="s">
+        <v>21</v>
+      </c>
+      <c r="K71" t="s">
+        <v>21</v>
+      </c>
+      <c r="L71" t="s">
+        <v>21</v>
+      </c>
+      <c r="M71" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="72" spans="1:19">
       <c r="A72" t="s">
@@ -3293,6 +4049,18 @@
       </c>
       <c r="I72" t="s">
         <v>266</v>
+      </c>
+      <c r="J72" t="s">
+        <v>21</v>
+      </c>
+      <c r="K72" t="s">
+        <v>21</v>
+      </c>
+      <c r="L72" t="s">
+        <v>21</v>
+      </c>
+      <c r="M72" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:19">
@@ -3340,6 +4108,18 @@
       <c r="I74" t="s">
         <v>21</v>
       </c>
+      <c r="J74" t="s">
+        <v>21</v>
+      </c>
+      <c r="K74" t="s">
+        <v>21</v>
+      </c>
+      <c r="L74" t="s">
+        <v>21</v>
+      </c>
+      <c r="M74" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="75" spans="1:19">
       <c r="D75" t="s">
@@ -3360,6 +4140,18 @@
       <c r="I75" t="s">
         <v>21</v>
       </c>
+      <c r="J75" t="s">
+        <v>21</v>
+      </c>
+      <c r="K75" t="s">
+        <v>21</v>
+      </c>
+      <c r="L75" t="s">
+        <v>21</v>
+      </c>
+      <c r="M75" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="76" spans="1:19">
       <c r="C76" t="s">
@@ -3381,6 +4173,18 @@
         <v>226</v>
       </c>
       <c r="I76" t="s">
+        <v>21</v>
+      </c>
+      <c r="J76" t="s">
+        <v>21</v>
+      </c>
+      <c r="K76" t="s">
+        <v>21</v>
+      </c>
+      <c r="L76" t="s">
+        <v>21</v>
+      </c>
+      <c r="M76" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3410,6 +4214,18 @@
         <v>251</v>
       </c>
       <c r="I77" t="s">
+        <v>21</v>
+      </c>
+      <c r="J77" t="s">
+        <v>21</v>
+      </c>
+      <c r="K77" t="s">
+        <v>21</v>
+      </c>
+      <c r="L77" t="s">
+        <v>21</v>
+      </c>
+      <c r="M77" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>